<commit_message>
Se generan versiones 1.0.3 y 1.0.4, aplicacion con todas las validaciones y desarrollo del normalizador de direccion
</commit_message>
<xml_diff>
--- a/documentacion/Requerimientos/29052022_Mockups Recuento .xlsx
+++ b/documentacion/Requerimientos/29052022_Mockups Recuento .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kmilo\Downloads\MAC2\DANE\DANE - Censo Economico\CE - Recuento\Entrega 2022\Ajuste 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Dane\2022\repo\dane_recuento_new_2022_personal\documentacion\Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6811516D-B62A-4A23-AB1A-493BD71BABE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D329C5-D889-4A46-81ED-F2D8CDE5F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53DC75AA-5F74-429E-8C5F-97EB90C51FDB}"/>
+    <workbookView xWindow="28530" yWindow="11090" windowWidth="10800" windowHeight="5840" xr2:uid="{53DC75AA-5F74-429E-8C5F-97EB90C51FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="CAP_I_UBICACION(UC-Edif-UE)" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'CAP_I_UBICACION(UC-Edif-UE)'!#REF!</definedName>
@@ -151,11 +150,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,7 +180,7 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>137160</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>26836</xdr:rowOff>
+      <xdr:rowOff>30011</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2240757" cy="2782625"/>
     <xdr:pic>
@@ -205,7 +204,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22113240" y="6610516"/>
+          <a:off x="7026910" y="7034855"/>
           <a:ext cx="2240757" cy="2782625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -241,8 +240,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="556260" y="765799"/>
-          <a:ext cx="2439307" cy="12807849"/>
+          <a:off x="536331" y="798086"/>
+          <a:ext cx="2352800" cy="13344375"/>
           <a:chOff x="556260" y="994399"/>
           <a:chExt cx="2439307" cy="12807849"/>
         </a:xfrm>
@@ -332,8 +331,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20465934" y="13451379"/>
-          <a:ext cx="3706784" cy="6295505"/>
+          <a:off x="19708867" y="14012572"/>
+          <a:ext cx="3592484" cy="6559030"/>
           <a:chOff x="8093528" y="1909354"/>
           <a:chExt cx="3703321" cy="6363789"/>
         </a:xfrm>
@@ -610,8 +609,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="24642584" y="13429608"/>
-          <a:ext cx="3943896" cy="6295505"/>
+          <a:off x="23768042" y="13990801"/>
+          <a:ext cx="3810546" cy="6559030"/>
           <a:chOff x="12262756" y="1887583"/>
           <a:chExt cx="3946073" cy="6363789"/>
         </a:xfrm>
@@ -955,8 +954,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="29066736" y="13429606"/>
-          <a:ext cx="5070963" cy="9003279"/>
+          <a:off x="28055034" y="13990799"/>
+          <a:ext cx="4910943" cy="9373484"/>
           <a:chOff x="8692241" y="1330431"/>
           <a:chExt cx="5104907" cy="8867504"/>
         </a:xfrm>
@@ -1306,8 +1305,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="34652296" y="13429212"/>
-          <a:ext cx="3951516" cy="6289800"/>
+          <a:off x="33480574" y="13990405"/>
+          <a:ext cx="3837216" cy="6556500"/>
           <a:chOff x="12316691" y="8465127"/>
           <a:chExt cx="3975761" cy="6220528"/>
         </a:xfrm>
@@ -3421,8 +3420,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14507095" y="640080"/>
-          <a:ext cx="2457319" cy="13405375"/>
+          <a:off x="13949516" y="669192"/>
+          <a:ext cx="2370373" cy="13967936"/>
           <a:chOff x="14507095" y="640080"/>
           <a:chExt cx="2457319" cy="13405375"/>
         </a:xfrm>
@@ -5772,31 +5771,6 @@
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="1. DatosGenerales"/>
-      <sheetName val="2. DescripciónDeFuncionalidades"/>
-      <sheetName val="3. DiagramaDeFlujo"/>
-      <sheetName val="4. EspecificaciónParaOE_Ubica_I"/>
-      <sheetName val="Perfiles"/>
-      <sheetName val="Hoja1"/>
-      <sheetName val="Hoja2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6104,16 +6078,16 @@
   </sheetPr>
   <dimension ref="C2:BE141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" workbookViewId="0">
-      <selection activeCell="BE2" sqref="BE2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A71" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="72" workbookViewId="0">
+      <selection activeCell="AR41" sqref="AR41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="74" width="3.77734375" customWidth="1"/>
+    <col min="1" max="74" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:57" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:57" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6121,29 +6095,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:57" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:57" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="3:57" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:57" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E4" s="2"/>
     </row>
-    <row r="14" spans="3:57" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:57" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:57" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:57" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="46" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6155,16 +6129,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2375E308-B8E5-44D0-B8A0-75C84A6552DB}">
   <dimension ref="C3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="BE2" sqref="BE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6186,67 +6160,67 @@
       <selection activeCell="BE2" sqref="BE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
-    <row r="15" spans="2:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>